<commit_message>
j'avais pas tout push
</commit_message>
<xml_diff>
--- a/doc/Question 1.xlsx
+++ b/doc/Question 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/a2d04f23f7faf3ef/Bureau/PROFESSIONAL/CANADA/5_Cours/H25_MEC8211/04_Devoir 3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02 - Etudes\05 - ETS\02 - H25\01 - Cours\MEC8211\03 - Devoirs\3\MEC8211_devoir_3\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{475A76FD-E0C6-467C-8979-08E67E811393}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013AD1A-CB7C-496C-841D-6F8C2EE5710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{B6386771-AB82-4E58-B1A6-EFBB55CE55B7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6386771-AB82-4E58-B1A6-EFBB55CE55B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
   <si>
     <t>seed = 3</t>
   </si>
@@ -91,12 +91,73 @@
   <si>
     <t>r23</t>
   </si>
+  <si>
+    <t>p obs</t>
+  </si>
+  <si>
+    <t>p formel</t>
+  </si>
+  <si>
+    <t>&lt;10%</t>
+  </si>
+  <si>
+    <t>GCI</t>
+  </si>
+  <si>
+    <t>critère GCI</t>
+  </si>
+  <si>
+    <t>microns</t>
+  </si>
+  <si>
+    <t>fh</t>
+  </si>
+  <si>
+    <t>u_num</t>
+  </si>
+  <si>
+    <t>QUESTION A</t>
+  </si>
+  <si>
+    <t>u_input</t>
+  </si>
+  <si>
+    <t>QUESTION D</t>
+  </si>
+  <si>
+    <t>u_D</t>
+  </si>
+  <si>
+    <t>u_val</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>E-ku_val</t>
+  </si>
+  <si>
+    <t>E+ku_val</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.0000%"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -122,15 +183,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3065,23 +3130,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809CF80D-8E3D-433E-8056-7C6649D3A18F}">
-  <dimension ref="A2:M25"/>
+  <dimension ref="A2:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="I24" sqref="I24"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="95" workbookViewId="0">
+      <selection activeCell="C43" sqref="C43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.81640625" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" customWidth="1"/>
-    <col min="6" max="6" width="15.90625" customWidth="1"/>
-    <col min="8" max="8" width="9.26953125" customWidth="1"/>
-    <col min="9" max="9" width="11.36328125" customWidth="1"/>
+    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.77734375" customWidth="1"/>
+    <col min="5" max="5" width="13.21875" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="8" max="8" width="9.21875" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3089,7 +3156,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3124,7 +3191,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4">
         <v>25</v>
       </c>
@@ -3163,7 +3230,7 @@
         <v>0.33512511584800764</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5">
         <v>50</v>
       </c>
@@ -3202,7 +3269,7 @@
         <v>0.33512511584800764</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6">
         <v>75</v>
       </c>
@@ -3241,7 +3308,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3284,7 +3351,7 @@
         <v>0.83089280197713844</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8">
         <v>115</v>
       </c>
@@ -3323,7 +3390,7 @@
         <v>0.31133765832561094</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9">
         <v>125</v>
       </c>
@@ -3362,7 +3429,7 @@
         <v>0.25523632993512496</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B10">
         <v>135</v>
       </c>
@@ -3401,7 +3468,7 @@
         <v>0.21390176088971233</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B11">
         <v>150</v>
       </c>
@@ -3440,7 +3507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B12">
         <v>160</v>
       </c>
@@ -3479,7 +3546,7 @@
         <v>6.0240963855421742E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B13">
         <v>175</v>
       </c>
@@ -3518,7 +3585,7 @@
         <v>0.14080939141180207</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3560,7 +3627,7 @@
         <v>0.18560395427865284</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B15">
         <v>225</v>
       </c>
@@ -3599,7 +3666,7 @@
         <v>0.2936051899907326</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B16">
         <v>250</v>
       </c>
@@ -3638,7 +3705,7 @@
         <v>0.20753784368242112</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B17">
         <v>300</v>
       </c>
@@ -3677,7 +3744,7 @@
         <v>0.24448563484708141</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B18">
         <v>325</v>
       </c>
@@ -3716,7 +3783,7 @@
         <v>0.1457522397281438</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B19">
         <v>350</v>
       </c>
@@ -3755,7 +3822,7 @@
         <v>0.18214396045721251</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3796,7 +3863,7 @@
         <v>0.23768921841210905</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -3805,7 +3872,7 @@
         <v>21.266500000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -3821,7 +3888,7 @@
         <v>1.0769230769230769</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B25" t="s">
         <v>15</v>
       </c>
@@ -3835,6 +3902,145 @@
       <c r="E25" s="1">
         <f>C19/C20</f>
         <v>1.142857142857143</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="3">
+        <f>(LN((E25^2-1)*(C23-C24)/(C24-C25)+E25^2))/LN(E25*E24)</f>
+        <v>1.9741543754497455</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>22</v>
+      </c>
+      <c r="B30" s="2">
+        <f>ABS((B29-B28)/B28)</f>
+        <v>1.292281227512726E-2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="3">
+        <f>1.25/(E25^B28-1)*ABS(C24-C25)</f>
+        <v>0.36709166666666659</v>
+      </c>
+      <c r="C31" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>24</v>
+      </c>
+      <c r="B32">
+        <f>C25</f>
+        <v>21.415299999999998</v>
+      </c>
+      <c r="C32" t="s">
+        <v>23</v>
+      </c>
+      <c r="D32" s="1"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="3">
+        <f>B31/2</f>
+        <v>0.1835458333333333</v>
+      </c>
+      <c r="C33" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>27</v>
+      </c>
+      <c r="B36">
+        <v>2.6850000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>29</v>
+      </c>
+      <c r="B37">
+        <v>17.7789</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>30</v>
+      </c>
+      <c r="B38">
+        <f>SQRT(B33^2+B36^2+B37^2)</f>
+        <v>17.981440411794992</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>31</v>
+      </c>
+      <c r="B40">
+        <v>-58.604999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>33</v>
+      </c>
+      <c r="B42">
+        <f>B40-B41*B38</f>
+        <v>-94.567880823589974</v>
+      </c>
+      <c r="C42">
+        <f>B41*B38</f>
+        <v>35.962880823589984</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43">
+        <f>B40+B41*B38</f>
+        <v>-22.642119176410013</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
modif pour le calcul de p observé
</commit_message>
<xml_diff>
--- a/doc/Question 1.xlsx
+++ b/doc/Question 1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\02 - Etudes\05 - ETS\02 - H25\01 - Cours\MEC8211\03 - Devoirs\3\MEC8211_devoir_3\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\OneDrive\Documentos\GitHub\MEC8211_devoir_3\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2013AD1A-CB7C-496C-841D-6F8C2EE5710B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0553DDB-41ED-40CF-B77C-91E33197ECC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B6386771-AB82-4E58-B1A6-EFBB55CE55B7}"/>
+    <workbookView xWindow="15645" yWindow="1350" windowWidth="28800" windowHeight="15345" xr2:uid="{B6386771-AB82-4E58-B1A6-EFBB55CE55B7}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="37">
   <si>
     <t>seed = 3</t>
   </si>
@@ -142,13 +142,19 @@
   <si>
     <t>E+ku_val</t>
   </si>
+  <si>
+    <t>N=115,125,135</t>
+  </si>
+  <si>
+    <t>N=75,100,115</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="0.0000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -187,15 +193,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="Pourcentage" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -213,7 +218,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -946,7 +951,7 @@
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="fr-FR"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -2814,7 +2819,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -3130,25 +3135,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{809CF80D-8E3D-433E-8056-7C6649D3A18F}">
-  <dimension ref="A2:M43"/>
+  <dimension ref="A2:M128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="95" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="95" workbookViewId="0">
+      <selection activeCell="K30" sqref="K30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.77734375" customWidth="1"/>
-    <col min="5" max="5" width="13.21875" customWidth="1"/>
-    <col min="6" max="6" width="15.88671875" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" customWidth="1"/>
-    <col min="9" max="9" width="11.33203125" customWidth="1"/>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="15.85546875" customWidth="1"/>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -3156,7 +3161,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>1</v>
       </c>
@@ -3191,7 +3196,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>25</v>
       </c>
@@ -3230,7 +3235,7 @@
         <v>0.33512511584800764</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>50</v>
       </c>
@@ -3269,7 +3274,7 @@
         <v>0.33512511584800764</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>75</v>
       </c>
@@ -3308,7 +3313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -3351,7 +3356,7 @@
         <v>0.83089280197713844</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>115</v>
       </c>
@@ -3390,7 +3395,7 @@
         <v>0.31133765832561094</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>125</v>
       </c>
@@ -3429,7 +3434,7 @@
         <v>0.25523632993512496</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>135</v>
       </c>
@@ -3468,7 +3473,7 @@
         <v>0.21390176088971233</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>150</v>
       </c>
@@ -3507,7 +3512,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>160</v>
       </c>
@@ -3546,7 +3551,7 @@
         <v>6.0240963855421742E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>175</v>
       </c>
@@ -3585,7 +3590,7 @@
         <v>0.14080939141180207</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
@@ -3627,7 +3632,7 @@
         <v>0.18560395427865284</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>225</v>
       </c>
@@ -3666,7 +3671,7 @@
         <v>0.2936051899907326</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>250</v>
       </c>
@@ -3705,7 +3710,7 @@
         <v>0.20753784368242112</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>300</v>
       </c>
@@ -3744,7 +3749,7 @@
         <v>0.24448563484708141</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>325</v>
       </c>
@@ -3783,7 +3788,7 @@
         <v>0.1457522397281438</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>350</v>
       </c>
@@ -3822,7 +3827,7 @@
         <v>0.18214396045721251</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>12</v>
       </c>
@@ -3863,7 +3868,19 @@
         <v>0.23768921841210905</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>36</v>
+      </c>
+      <c r="I22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22">
+        <f>C6/C7</f>
+        <v>1.3333333333333335</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>13</v>
       </c>
@@ -3871,8 +3888,15 @@
         <f>I18</f>
         <v>21.266500000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="I23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="1">
+        <f>C7/C8</f>
+        <v>1.1499999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>14</v>
       </c>
@@ -3888,7 +3912,7 @@
         <v>1.0769230769230769</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>15</v>
       </c>
@@ -3904,29 +3928,63 @@
         <v>1.142857142857143</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G26" t="e">
+        <f>(I6-I5)/(I5-I4)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="I26" s="1">
+        <f>LN(($J$22^1-1)*$G$30+$J$22^1)/LN($J$22*$J$23)</f>
+        <v>1.068552020079766</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G27">
+        <f t="shared" ref="G27:G50" si="12">(I7-I6)/(I6-I5)</f>
+        <v>-0.2543443917851515</v>
+      </c>
+      <c r="I27" s="1">
+        <f>LN(($J$22^I26-1)*$G$30+$J$22^I26)/LN($J$22*$J$23)</f>
+        <v>1.1359114355584343</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>19</v>
       </c>
       <c r="B28">
         <v>2</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G28">
+        <f t="shared" si="12"/>
+        <v>3.0723419802703429</v>
+      </c>
+      <c r="I28" s="1">
+        <f t="shared" ref="I28:I91" si="13">LN(($J$22^I27-1)*$G$30+$J$22^I27)/LN($J$22*$J$23)</f>
+        <v>1.20151475578686</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>18</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29">
         <f>(LN((E25^2-1)*(C23-C24)/(C24-C25)+E25^2))/LN(E25*E24)</f>
         <v>1.9741543754497455</v>
       </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G29">
+        <f t="shared" si="12"/>
+        <v>0.10797954572482077</v>
+      </c>
+      <c r="I29" s="1">
+        <f t="shared" si="13"/>
+        <v>1.2648711160264554</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>22</v>
       </c>
@@ -3937,20 +3995,39 @@
       <c r="C30" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="F30" t="s">
+        <v>35</v>
+      </c>
+      <c r="G30">
+        <f>(I10-I9)/(I9-I8)</f>
+        <v>0.7367841409691549</v>
+      </c>
+      <c r="I30" s="1">
+        <f t="shared" si="13"/>
+        <v>1.3255722079766572</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>21</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31">
         <f>1.25/(E25^B28-1)*ABS(C24-C25)</f>
         <v>0.36709166666666659</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="G31">
+        <f t="shared" si="12"/>
+        <v>5.1748878923766446</v>
+      </c>
+      <c r="I31" s="1">
+        <f t="shared" si="13"/>
+        <v>1.3832968405823454</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>24</v>
       </c>
@@ -3962,41 +4039,91 @@
         <v>23</v>
       </c>
       <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G32">
+        <f t="shared" si="12"/>
+        <v>-0.28162911611785169</v>
+      </c>
+      <c r="I32" s="1">
+        <f t="shared" si="13"/>
+        <v>1.4378106727658189</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>25</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33">
         <f>B31/2</f>
         <v>0.1835458333333333</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G33">
+        <f t="shared" si="12"/>
+        <v>1.3374358974359122</v>
+      </c>
+      <c r="I33" s="1">
+        <f t="shared" si="13"/>
+        <v>1.4889619747326004</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G34">
+        <f t="shared" si="12"/>
+        <v>0.5559815950920024</v>
+      </c>
+      <c r="I34" s="1">
+        <f t="shared" si="13"/>
+        <v>1.5366744264631809</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G35">
+        <f t="shared" si="12"/>
+        <v>2.4110344827587031</v>
+      </c>
+      <c r="I35" s="1">
+        <f t="shared" si="13"/>
+        <v>1.580937973795012</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>27</v>
       </c>
       <c r="B36">
         <v>2.6850000000000001</v>
       </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G36">
+        <f t="shared" si="12"/>
+        <v>-0.79691075514874865</v>
+      </c>
+      <c r="I36" s="1">
+        <f t="shared" si="13"/>
+        <v>1.6217986713625512</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>29</v>
       </c>
       <c r="B37">
         <v>17.7789</v>
       </c>
-    </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G37">
+        <f>(I17-I16)/(I16-I15)</f>
+        <v>-0.42928930366117585</v>
+      </c>
+      <c r="I37" s="1">
+        <f t="shared" si="13"/>
+        <v>1.6593482880906616</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>30</v>
       </c>
@@ -4004,24 +4131,54 @@
         <f>SQRT(B33^2+B36^2+B37^2)</f>
         <v>17.981440411794992</v>
       </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G38">
+        <f t="shared" si="12"/>
+        <v>-2.6722408026754731</v>
+      </c>
+      <c r="I38" s="1">
+        <f t="shared" si="13"/>
+        <v>1.6937142708982453</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G39">
+        <f t="shared" si="12"/>
+        <v>-0.36858573216519092</v>
+      </c>
+      <c r="I39" s="1">
+        <f t="shared" si="13"/>
+        <v>1.7250504831753337</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>31</v>
       </c>
       <c r="B40">
         <v>-58.604999999999997</v>
       </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="G40">
+        <f>(I20-I19)/(I19-I18)</f>
+        <v>1.5263157894737445</v>
+      </c>
+      <c r="I40" s="1">
+        <f t="shared" si="13"/>
+        <v>1.7535289743311244</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>32</v>
       </c>
       <c r="B41">
         <v>2</v>
       </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I41" s="1">
+        <f>LN(($J$22^I40-1)*$G$30+$J$22^I40)/LN($J$22*$J$23)</f>
+        <v>1.7793329046481563</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>33</v>
       </c>
@@ -4033,8 +4190,12 @@
         <f>B41*B38</f>
         <v>35.962880823589984</v>
       </c>
-    </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="I42" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8026506486601079</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>34</v>
       </c>
@@ -4042,6 +4203,475 @@
         <f>B40+B41*B38</f>
         <v>-22.642119176410013</v>
       </c>
+      <c r="I43" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8236710287673061</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I44" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8425795848138635</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I45" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8595557598481809</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I46" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8747708721957128</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I47" s="1">
+        <f t="shared" si="13"/>
+        <v>1.8883867447231542</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="I48" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9005548699753232</v>
+      </c>
+    </row>
+    <row r="49" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I49" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9114160017652719</v>
+      </c>
+    </row>
+    <row r="50" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I50" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9211000776189433</v>
+      </c>
+    </row>
+    <row r="51" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I51" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9297263907062134</v>
+      </c>
+    </row>
+    <row r="52" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I52" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9374039435485892</v>
+      </c>
+    </row>
+    <row r="53" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I53" s="1">
+        <f>LN(($J$22^I52-1)*$G$30+$J$22^I52)/LN($J$22*$J$23)</f>
+        <v>1.9442319282996512</v>
+      </c>
+    </row>
+    <row r="54" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I54" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9503002894560419</v>
+      </c>
+    </row>
+    <row r="55" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I55" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9556903343811096</v>
+      </c>
+    </row>
+    <row r="56" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I56" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9604753650445927</v>
+      </c>
+    </row>
+    <row r="57" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I57" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9647213110103796</v>
+      </c>
+    </row>
+    <row r="58" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I58" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9684873490901638</v>
+      </c>
+    </row>
+    <row r="59" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I59" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9718264993880983</v>
+      </c>
+    </row>
+    <row r="60" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I60" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9747861908535327</v>
+      </c>
+    </row>
+    <row r="61" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I61" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9774087920882286</v>
+      </c>
+    </row>
+    <row r="62" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I62" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9797321051581589</v>
+      </c>
+    </row>
+    <row r="63" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I63" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9817898216576972</v>
+      </c>
+    </row>
+    <row r="64" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I64" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9836119413677202</v>
+      </c>
+    </row>
+    <row r="65" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I65" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9852251546243018</v>
+      </c>
+    </row>
+    <row r="66" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I66" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9866531900418025</v>
+      </c>
+    </row>
+    <row r="67" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I67" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9879171295706803</v>
+      </c>
+    </row>
+    <row r="68" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I68" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9890356930624882</v>
+      </c>
+    </row>
+    <row r="69" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I69" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9900254945991362</v>
+      </c>
+    </row>
+    <row r="70" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I70" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9909012728496236</v>
+      </c>
+    </row>
+    <row r="71" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I71" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9916760976677079</v>
+      </c>
+    </row>
+    <row r="72" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I72" s="1">
+        <f t="shared" si="13"/>
+        <v>1.992361555055947</v>
+      </c>
+    </row>
+    <row r="73" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I73" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9929679125085409</v>
+      </c>
+    </row>
+    <row r="74" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I74" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9935042666175189</v>
+      </c>
+    </row>
+    <row r="75" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I75" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9939786746915451</v>
+      </c>
+    </row>
+    <row r="76" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I76" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9943982719994202</v>
+      </c>
+    </row>
+    <row r="77" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I77" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9947693761151555</v>
+      </c>
+    </row>
+    <row r="78" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I78" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9950975797109398</v>
+      </c>
+    </row>
+    <row r="79" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I79" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9953878330202435</v>
+      </c>
+    </row>
+    <row r="80" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I80" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9956445170767387</v>
+      </c>
+    </row>
+    <row r="81" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I81" s="1">
+        <f t="shared" si="13"/>
+        <v>1.995871508726315</v>
+      </c>
+    </row>
+    <row r="82" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I82" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9960722383093343</v>
+      </c>
+    </row>
+    <row r="83" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I83" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9962497408184807</v>
+      </c>
+    </row>
+    <row r="84" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I84" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9964067012537272</v>
+      </c>
+    </row>
+    <row r="85" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I85" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9965454948198071</v>
+      </c>
+    </row>
+    <row r="86" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I86" s="1">
+        <f t="shared" si="13"/>
+        <v>1.996668222542638</v>
+      </c>
+    </row>
+    <row r="87" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I87" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9967767428189407</v>
+      </c>
+    </row>
+    <row r="88" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I88" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9968726993572872</v>
+      </c>
+    </row>
+    <row r="89" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I89" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9969575459185394</v>
+      </c>
+    </row>
+    <row r="90" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I90" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9970325682185623</v>
+      </c>
+    </row>
+    <row r="91" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I91" s="1">
+        <f t="shared" si="13"/>
+        <v>1.9970989033157844</v>
+      </c>
+    </row>
+    <row r="92" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I92" s="1">
+        <f t="shared" ref="I92:I128" si="14">LN(($J$22^I91-1)*$G$30+$J$22^I91)/LN($J$22*$J$23)</f>
+        <v>1.9971575567701423</v>
+      </c>
+    </row>
+    <row r="93" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I93" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9972094178278068</v>
+      </c>
+    </row>
+    <row r="94" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I94" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9972552728574404</v>
+      </c>
+    </row>
+    <row r="95" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I95" s="1">
+        <f t="shared" si="14"/>
+        <v>1.997295817238232</v>
+      </c>
+    </row>
+    <row r="96" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I96" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9973316658772451</v>
+      </c>
+    </row>
+    <row r="97" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I97" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9973633625134641</v>
+      </c>
+    </row>
+    <row r="98" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I98" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9973913879479819</v>
+      </c>
+    </row>
+    <row r="99" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I99" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9974161673238664</v>
+      </c>
+    </row>
+    <row r="100" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I100" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9974380765651198</v>
+      </c>
+    </row>
+    <row r="101" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I101" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9974574480716187</v>
+      </c>
+    </row>
+    <row r="102" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I102" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9974745757558077</v>
+      </c>
+    </row>
+    <row r="103" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I103" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9974897194970815</v>
+      </c>
+    </row>
+    <row r="104" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I104" s="1">
+        <f t="shared" si="14"/>
+        <v>1.99750310908106</v>
+      </c>
+    </row>
+    <row r="105" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I105" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975149476832288</v>
+      </c>
+    </row>
+    <row r="106" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I106" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975254149495738</v>
+      </c>
+    </row>
+    <row r="107" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I107" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975346697207794</v>
+      </c>
+    </row>
+    <row r="108" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I108" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975428524411778</v>
+      </c>
+    </row>
+    <row r="109" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I109" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975500872889067</v>
+      </c>
+    </row>
+    <row r="110" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I110" s="1">
+        <f t="shared" si="14"/>
+        <v>1.997556484059503</v>
+      </c>
+    </row>
+    <row r="111" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I111" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975621398314594</v>
+      </c>
+    </row>
+    <row r="112" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I112" s="1">
+        <f t="shared" si="14"/>
+        <v>1.9975671404389606</v>
+      </c>
+    </row>
+    <row r="113" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I113" s="1">
+        <f t="shared" si="14"/>
+        <v>1.997571561774111</v>
+      </c>
+    </row>
+    <row r="114" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I114" s="1"/>
+    </row>
+    <row r="115" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I115" s="1"/>
+    </row>
+    <row r="116" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I116" s="1"/>
+    </row>
+    <row r="117" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I117" s="1"/>
+    </row>
+    <row r="118" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I118" s="1"/>
+    </row>
+    <row r="119" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I119" s="1"/>
+    </row>
+    <row r="120" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I120" s="1"/>
+    </row>
+    <row r="121" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I121" s="1"/>
+    </row>
+    <row r="122" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I122" s="1"/>
+    </row>
+    <row r="123" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I123" s="1"/>
+    </row>
+    <row r="124" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I124" s="1"/>
+    </row>
+    <row r="125" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I125" s="1"/>
+    </row>
+    <row r="126" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I126" s="1"/>
+    </row>
+    <row r="127" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I127" s="1"/>
+    </row>
+    <row r="128" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I128" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>